<commit_message>
docs and pics after presentation making sure its the latest version
</commit_message>
<xml_diff>
--- a/docs/results FP.xlsx
+++ b/docs/results FP.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74203a780c3e4554/Documents/GitHub/MThesis-Foosball/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E7B634-BDBA-4A38-B627-B64D6A6F5F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{43E7B634-BDBA-4A38-B627-B64D6A6F5F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E9989F3-115F-4EBA-9A6E-0C8A74EA145D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{D24CE1DE-49F9-4153-A5A2-50A6414FF0B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D24CE1DE-49F9-4153-A5A2-50A6414FF0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
   <si>
     <t>Continuous</t>
   </si>
@@ -69,6 +70,15 @@
   </si>
   <si>
     <t>Av. Time</t>
+  </si>
+  <si>
+    <t>av</t>
+  </si>
+  <si>
+    <t>Average Time for a Succesfull Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -126,7 +136,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -188,7 +198,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -253,13 +263,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>44</c:v>
@@ -330,13 +340,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>72</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>27</c:v>
@@ -410,10 +420,10 @@
                   <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>58</c:v>
@@ -484,13 +494,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>76</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>67</c:v>
@@ -561,7 +571,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="879124799"/>
@@ -620,7 +630,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="879122399"/>
@@ -662,7 +672,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -692,7 +702,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="LID4096"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -706,7 +716,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -773,7 +783,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1146,7 +1156,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="879125759"/>
@@ -1205,7 +1215,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="879121919"/>
@@ -1247,7 +1257,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1277,7 +1287,1434 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Normalised Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of Succesfull Passes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Continuous</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Non_factror</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Corner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rythmic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-2.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-12.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F810-4550-B529-757B21F8ADC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DCCM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Non_factror</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Corner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rythmic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$25:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-4.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F810-4550-B529-757B21F8ADC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DCCS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Non_factror</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Corner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rythmic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F810-4550-B529-757B21F8ADC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Discrete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Non_factror</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Corner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rythmic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F810-4550-B529-757B21F8ADC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1243695823"/>
+        <c:axId val="1243693903"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1243695823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1243693903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1243693903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1243695823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Continuous</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Non_factror</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Corner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rythmic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.70998159999999988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.33726659999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.2763125999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67850640000000029</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64505440000000025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9A74-419C-898E-2D09A6098038}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DCCM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Non_factror</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Corner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rythmic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.27804779999999951</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76142079999999979</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.23623219999999989</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.3750492000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.42818719999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9A74-419C-898E-2D09A6098038}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DCCS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Non_factror</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Corner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rythmic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.74208980000000047</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.19596020000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65293880000000026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.79180120000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.40726719999999972</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9A74-419C-898E-2D09A6098038}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Discrete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Non_factror</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Corner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rythmic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.2975509999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.580775</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.46217199999999981</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.29309899999999978</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.52795299999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9A74-419C-898E-2D09A6098038}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="916251552"/>
+        <c:axId val="916258272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="916251552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="916258272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="916258272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="916251552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Time for a Succesfull Pass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$31:$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Continuous</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DCCM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DCCS</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Discrete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$31:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.2815966000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3670502000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1077252</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88701660000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0376-4014-910C-717987C6870E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="873829872"/>
+        <c:axId val="873830832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="873829872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873830832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="873830832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873829872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1368,6 +2805,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1872,6 +3429,1515 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2414,16 +5480,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>557212</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>150812</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>149225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>92075</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2448,7 +5514,119 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>92074</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{598AE482-6309-328D-9CA7-F9942BDFDCA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>403225</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>98425</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A408BD0D-90DC-CD07-0323-0B882EB94ED7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>511175</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82485EA6-8158-2F54-9F17-C61C7B756CBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2748,19 +5926,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3591D6-72B1-4FFA-BFF1-BFC17283493E}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2780,18 +5958,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2">
+        <v>43</v>
+      </c>
+      <c r="D2">
         <v>44</v>
-      </c>
-      <c r="D2">
-        <v>42</v>
       </c>
       <c r="E2">
         <v>44</v>
@@ -2800,18 +5978,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E3">
         <v>27</v>
@@ -2820,7 +5998,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2828,10 +6006,10 @@
         <v>81</v>
       </c>
       <c r="C4">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>58</v>
@@ -2840,18 +6018,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C5">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D5">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5">
         <v>67</v>
@@ -2860,7 +6038,29 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <f>AVERAGE(B2:B5)</f>
+        <v>75.75</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:F6" si="0">AVERAGE(C2:C5)</f>
+        <v>46.25</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>56.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2879,8 +6079,11 @@
       <c r="F8" t="s">
         <v>8</v>
       </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2899,8 +6102,12 @@
       <c r="F9">
         <v>3.326651</v>
       </c>
+      <c r="G9">
+        <f>AVERAGE(B9:F9)</f>
+        <v>2.6815965999999998</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2919,8 +6126,12 @@
       <c r="F10">
         <v>5.7388630000000003</v>
       </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G12" si="1">AVERAGE(B10:F10)</f>
+        <v>6.1670502000000003</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2939,8 +6150,12 @@
       <c r="F11">
         <v>5.2004580000000002</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>5.6077252</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2958,6 +6173,313 @@
       </c>
       <c r="F12">
         <v>1.842716</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>2.3706689999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <f>AVERAGE(B9:B12)</f>
+        <v>4.2099115000000005</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:F13" si="2">AVERAGE(C9:C12)</f>
+        <v>4.6590024999999997</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>4.1263157499999998</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>4.0113995000000005</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>4.0271720000000002</v>
+      </c>
+      <c r="G13">
+        <f>AVERAGE(G9:G12)</f>
+        <v>4.2067602500000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <f>B9-$G9</f>
+        <v>-0.70998159999999988</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:F16" si="3">C9-$G9</f>
+        <v>-0.33726659999999997</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>-0.2763125999999998</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>0.67850640000000029</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>0.64505440000000025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:F17" si="4">B10-$G10</f>
+        <v>0.27804779999999951</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="4"/>
+        <v>0.76142079999999979</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>-0.23623219999999989</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>-0.3750492000000003</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>-0.42818719999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ref="B18:F18" si="5">B11-$G11</f>
+        <v>0.74208980000000047</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="5"/>
+        <v>-0.19596020000000003</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="5"/>
+        <v>0.65293880000000026</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="5"/>
+        <v>-0.79180120000000009</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>-0.40726719999999972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ref="B19:F19" si="6">B12-$G12</f>
+        <v>-0.2975509999999999</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="6"/>
+        <v>1.580775</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="6"/>
+        <v>-0.46217199999999981</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>-0.29309899999999978</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="6"/>
+        <v>-0.52795299999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <f>B2-B$6</f>
+        <v>-2.75</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:F24" si="7">C2-C$6</f>
+        <v>-3.25</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="7"/>
+        <v>-12.5</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:F25" si="8">B3-B$6</f>
+        <v>-4.75</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="8"/>
+        <v>-4.25</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="8"/>
+        <v>-22</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26:F26" si="9">B4-B$6</f>
+        <v>5.25</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="9"/>
+        <v>6.75</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="9"/>
+        <v>5.5</v>
+      </c>
+      <c r="E26">
+        <f>E4-E$6</f>
+        <v>9</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ref="B27:F27" si="10">B5-B$6</f>
+        <v>2.25</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="10"/>
+        <v>4.5</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>1.2815966000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>4.3670502000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>3.1077252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>0.88701660000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>